<commit_message>
se agrego info en experiencia y educacion
</commit_message>
<xml_diff>
--- a/Modulo 1/planificacion.xlsx
+++ b/Modulo 1/planificacion.xlsx
@@ -64,9 +64,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,7 +372,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +400,9 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2">
+        <v>44582</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>

</xml_diff>